<commit_message>
test_photodiode done minor bug fixed
</commit_message>
<xml_diff>
--- a/tables/tablePhotodiode.xlsx
+++ b/tables/tablePhotodiode.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Godovova\MATLAB_Godovova\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\greatuniter\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBE3288-B73C-4ED5-A725-606533583849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="12360" windowHeight="9000" tabRatio="861" activeTab="1"/>
+    <workbookView xWindow="-17310" yWindow="1485" windowWidth="16200" windowHeight="9360" tabRatio="861" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
     <sheet name="Array" sheetId="2" r:id="rId2"/>
     <sheet name="Sample" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -227,7 +236,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,52 +413,12 @@
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="3"/>
-    <cellStyle name="Обычный 3" xfId="4"/>
-    <cellStyle name="Стиль 1" xfId="1"/>
-    <cellStyle name="Стиль 2" xfId="2"/>
+    <cellStyle name="Обычный 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Обычный 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Стиль 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Стиль 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -501,9 +470,9 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Стиль таблицы 1" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Стиль таблицы 1" pivot="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="5"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="4"/>
+    <tableStyle name="Стиль таблицы 1" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -779,7 +748,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -921,11 +890,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,11 +1367,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BT65"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>